<commit_message>
Test Excel data file. Currently contains 2 worksheets: CorePrices and Customers
</commit_message>
<xml_diff>
--- a/ExcelDataReader/Data/AutomatedTestData.xlsx
+++ b/ExcelDataReader/Data/AutomatedTestData.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Keith\iCloudDrive\Findel\Working\Web_Core Pricing Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ExcelDataReader\ExcelDataReader\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26535" windowHeight="12180" xr2:uid="{05B1F881-7DFD-46DC-8ADE-383D7CE28B32}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26535" windowHeight="12180" activeTab="1" xr2:uid="{05B1F881-7DFD-46DC-8ADE-383D7CE28B32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Core" sheetId="1" r:id="rId1"/>
+    <sheet name="CorePrices" sheetId="1" r:id="rId1"/>
+    <sheet name="Customers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Brand</t>
   </si>
@@ -51,16 +52,83 @@
   </si>
   <si>
     <t>G100051</t>
+  </si>
+  <si>
+    <t>A4570009485</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Keith Test 1</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>H1000051</t>
+  </si>
+  <si>
+    <t>HOP11111</t>
+  </si>
+  <si>
+    <t>HOP</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Price Group</t>
+  </si>
+  <si>
+    <t>Core Group</t>
+  </si>
+  <si>
+    <t>Header Discount</t>
+  </si>
+  <si>
+    <t>Keith.Manning@Findel-Education.co.uk</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>SXL</t>
+  </si>
+  <si>
+    <t>SCH</t>
+  </si>
+  <si>
+    <t>Web Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Malgun Gothic Semilight"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Malgun Gothic Semilight"/>
       <family val="2"/>
     </font>
@@ -82,13 +150,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -105,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3C73332-4D1D-4CB8-9FD9-F4B8CD29671B}" name="CorePrices" displayName="CorePrices" ref="A1:F3" totalsRowShown="0">
-  <autoFilter ref="A1:F3" xr:uid="{699E3DD9-72A2-4A12-AB80-48330BBE04AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3C73332-4D1D-4CB8-9FD9-F4B8CD29671B}" name="CorePrices" displayName="CorePrices" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{699E3DD9-72A2-4A12-AB80-48330BBE04AF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{16BA4F0D-5B98-431F-8648-E5E9579ADA1D}" name="Brand"/>
     <tableColumn id="2" xr3:uid="{491F7731-C0C8-4284-8C98-94B27D9806D2}" name="Material"/>
@@ -114,6 +185,23 @@
     <tableColumn id="4" xr3:uid="{3F9856A2-A072-44F9-9A2F-986ED346BE9B}" name="CorePrice"/>
     <tableColumn id="5" xr3:uid="{1FBD5C13-1F5F-420D-8174-2F7E033C593C}" name="Customer"/>
     <tableColumn id="6" xr3:uid="{C8E48D37-AEC8-4FB6-96FF-3B97B6228D33}" name="CoreGroup"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02E88B58-A6C7-4877-82C5-7D9FD230BC18}" name="Customers" displayName="Customers" ref="A1:H3" totalsRowShown="0">
+  <autoFilter ref="A1:H3" xr:uid="{61311000-9638-4DFB-B433-B0D0DCD1CCA5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D79B8D4C-AE06-485E-ACFF-7B5FED4E5280}" name="AccountNumber"/>
+    <tableColumn id="2" xr3:uid="{DB5A6C58-613C-4103-975C-6926276CCED9}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{5DC2F5BA-85CC-441F-BB70-E15934F6D456}" name="Brand"/>
+    <tableColumn id="4" xr3:uid="{5538B8DC-7243-4C84-A474-971CC9B5C1F7}" name="Email"/>
+    <tableColumn id="5" xr3:uid="{64273330-43B0-4DC6-8709-AB9E6A86E82E}" name="Web Password"/>
+    <tableColumn id="6" xr3:uid="{9B5FA328-048D-4985-BB81-431B86FD6F8A}" name="Price Group"/>
+    <tableColumn id="7" xr3:uid="{94128C28-432B-4C99-ABAF-2643848AF25F}" name="Core Group"/>
+    <tableColumn id="8" xr3:uid="{EA74F0FC-9AA8-4691-AEAB-1150173A6ECC}" name="Header Discount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -416,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D0058-1945-40FC-A16C-485F2FB18FBC}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -465,8 +553,11 @@
       <c r="D2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E2">
-        <v>4570009485</v>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -484,6 +575,26 @@
       </c>
       <c r="E3">
         <v>4570009485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D4">
+        <v>3.33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -492,4 +603,98 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC19B5A3-D18A-4367-93EC-5DF88B0A29A5}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4570009485</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6EA20767-3858-45DF-9F01-1A86CD5CE7D8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>